<commit_message>
Fix duplicate name in sugar kelp example
</commit_message>
<xml_diff>
--- a/examples/sugar kelp/traits.xlsx
+++ b/examples/sugar kelp/traits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djw64/OneDrive - Cornell University/T3/projects/ontology scripts/examples/sugar kelp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CC8B8C-5890-7944-9F8B-1F6443FC814C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EAE284-50F2-3940-A584-97C654B2260A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7400" yWindow="780" windowWidth="38780" windowHeight="23720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6500" yWindow="3080" windowWidth="33580" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="462">
   <si>
     <t>Scale ID</t>
   </si>
@@ -1416,6 +1416,9 @@
   </si>
   <si>
     <t>Weight of all individuals in all sampled subplots (1cm subsamples)</t>
+  </si>
+  <si>
+    <t>Sampled subplot count</t>
   </si>
 </sst>
 </file>
@@ -1910,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4815,7 +4818,7 @@
         <v>97</v>
       </c>
       <c r="O68" s="7" t="s">
-        <v>431</v>
+        <v>461</v>
       </c>
       <c r="P68" s="3" t="s">
         <v>449</v>
@@ -4825,7 +4828,7 @@
       </c>
       <c r="R68" t="str">
         <f t="shared" si="0"/>
-        <v>Subplot count|Sampled subplot count - Measurement|count</v>
+        <v>Sampled subplot count|Sampled subplot count - Measurement|count</v>
       </c>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.2">
@@ -5031,8 +5034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:XFD62"/>
+    <sheetView topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6488,7 +6491,7 @@
         <v>284</v>
       </c>
       <c r="B62" t="s">
-        <v>431</v>
+        <v>461</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>65</v>
@@ -6503,7 +6506,7 @@
         <v>407</v>
       </c>
       <c r="I62" t="s">
-        <v>431</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -6529,7 +6532,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>